<commit_message>
updates mainly for constructing the new nutrient lookup table.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/IMPACTcodeLookup.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/IMPACTcodeLookup.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-26920" yWindow="460" windowWidth="27360" windowHeight="14860" tabRatio="500"/>
+    <workbookView xWindow="4520" yWindow="2180" windowWidth="23040" windowHeight="14860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>IMPACT_code</t>
   </si>
@@ -134,15 +134,9 @@
     <t>c_Salmon</t>
   </si>
   <si>
-    <t>15076</t>
-  </si>
-  <si>
     <t>c_Tuna</t>
   </si>
   <si>
-    <t>15123</t>
-  </si>
-  <si>
     <t>clent</t>
   </si>
   <si>
@@ -275,9 +269,6 @@
     <t>cwhea</t>
   </si>
   <si>
-    <t>20076</t>
-  </si>
-  <si>
     <t>cyams</t>
   </si>
   <si>
@@ -345,6 +336,69 @@
   </si>
   <si>
     <t>c_OMarn</t>
+  </si>
+  <si>
+    <t>11973, 11043, 16001, 16014, 16016, 16022, 16024, 16027, 16037, 16040, 16042, 16047, 16049, 16071</t>
+  </si>
+  <si>
+    <t>09279, 09291, 09296, 09302, 09316, 09326</t>
+  </si>
+  <si>
+    <t>17168, 17224</t>
+  </si>
+  <si>
+    <t>04582, 04583</t>
+  </si>
+  <si>
+    <t>16087, 12104, 09193, 12036, 12021, 12023, 02024, 02033, 12160, 12012</t>
+  </si>
+  <si>
+    <t>15157, 15164, 15167, 15171, 15172, 15177, 35028, 90560</t>
+  </si>
+  <si>
+    <t>15003, 15008, 15008, 15010, 15025, 15053, 15060, 15079, 15081, 15083, 15085, 15115, 15234, 15236, 15261</t>
+  </si>
+  <si>
+    <t>15001, 15007, 15039, 15039, 15043, 15046, 15049, 15050, 15117, 15123, 15127</t>
+  </si>
+  <si>
+    <t>15015, 15020, 15025, 15028, 15028, 15031, 15033, 15038, 15055, 15065, 15091, 15091, 15095, 15101, , 15132, 15135, 15266, 15268</t>
+  </si>
+  <si>
+    <t>12078, 12087, 12097, 12061, 12155, 12151, 12120</t>
+  </si>
+  <si>
+    <t>20062, 20038, 20008, 20035, 20069</t>
+  </si>
+  <si>
+    <t>14355</t>
+  </si>
+  <si>
+    <t>11973, 11304, 16056, 16060, 16101, 16069, 16076</t>
+  </si>
+  <si>
+    <t>9037, 9089, 9094, 9111, 9125, 9132, 9135, 9139, 9148, 9150, 9153, 9154, 9159, 9181, 9200, 9206, 9214, 9218, 9221, 9226, 9265, 9266, 9268, 9273, 9274, 9298, 9404, 9421, 9436, 14262, 14263</t>
+  </si>
+  <si>
+    <t>9181, 9326, 11007, 11011, 11052, 11090, 11109, 11124, 11135, 11205, 11209, 11215, 11246, 11257, 11265, 11278, 11282, 11422, 11457, 11529, 11546, 11584, 11670, 11677, 11885, 16055, 16085, 20014</t>
+  </si>
+  <si>
+    <t>15136, 15139, 15143, 15144, 15145, 15147, 15149, 15154</t>
+  </si>
+  <si>
+    <t>02024</t>
+  </si>
+  <si>
+    <t>15236</t>
+  </si>
+  <si>
+    <t>15127</t>
+  </si>
+  <si>
+    <t>20072</t>
+  </si>
+  <si>
+    <t>IMPACT_conversion</t>
   </si>
 </sst>
 </file>
@@ -352,7 +406,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -416,61 +470,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,473 +779,532 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" style="9" customWidth="1"/>
-    <col min="2" max="2" width="6" style="6" customWidth="1"/>
+    <col min="1" max="1" width="17" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="C1" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="C7" s="10">
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="C9" s="10">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="B19" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B22" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B23" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B24" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B25" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B26" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B29" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B31" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="C31" s="10">
+        <v>72.900000000000006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B32" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B33" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B34" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B35" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="9" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B36" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B37" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B38" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B39" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B40" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="9" t="s">
+      <c r="B41" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B42" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
+      <c r="B43" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="8" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
+      <c r="B44" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B45" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="14" t="s">
+      <c r="C45" s="10">
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="15"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
+      <c r="B46" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="6" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="B47" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B48" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="B49" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="8"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="16" t="s">
+      <c r="B50" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="17"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="9" t="s">
+      <c r="B51" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
+      <c r="B52" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
+      <c r="B53" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="9" t="s">
+      <c r="B54" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+      <c r="B55" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
+      <c r="B56" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B54" s="8"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="9" t="s">
+      <c r="B57" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="7" t="s">
+      <c r="B58" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B56" s="8"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="7" t="s">
+      <c r="B59" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B57" s="8"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
+      <c r="B60" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B58" s="8"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
+      <c r="B61" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B59" s="8"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B60" s="8"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B61" s="8"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B62" s="8"/>
+      <c r="B62" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A range of changes from dealing with naming conventions to development of diversity measures.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/IMPACTcodeLookup.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/IMPACTcodeLookup.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="2180" windowWidth="23040" windowHeight="14860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>IMPACT_code</t>
   </si>
@@ -389,9 +390,6 @@
     <t>11088, 11973, 11304, 16056, 16060, 16101, 16069, 16076</t>
   </si>
   <si>
-    <t>12104, 09193, 12021, 12023, 02024, 02033, 12160, 12012</t>
-  </si>
-  <si>
     <t>09003, 09252, 09296, 09021, 09063, 09070, 09236, 09279, 09316, 09107, 09084, 09050, 09078, 09326</t>
   </si>
   <si>
@@ -399,6 +397,12 @@
   </si>
   <si>
     <t>19165</t>
+  </si>
+  <si>
+    <t>IMPACT conversion for poultry removed because the USDA edible share correction is for removing bones.</t>
+  </si>
+  <si>
+    <t>12104, 09193, 12021, 12023, 02033, 12160, 12012</t>
   </si>
 </sst>
 </file>
@@ -408,7 +412,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -442,6 +446,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -470,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
@@ -501,6 +511,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,9 +880,6 @@
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="10">
-        <v>61</v>
-      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -886,7 +894,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="10">
         <v>82</v>
@@ -1129,6 +1137,9 @@
       <c r="B40" s="2" t="s">
         <v>111</v>
       </c>
+      <c r="C40" s="11">
+        <v>66.67</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
@@ -1237,7 +1248,7 @@
         <v>92</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1245,7 +1256,7 @@
         <v>93</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1253,7 +1264,7 @@
         <v>94</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1316,4 +1327,22 @@
     <ignoredError sqref="B2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
A bunch of cleaned up files
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/IMPACTcodeLookup.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/IMPACTcodeLookup.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="57720" yWindow="-8160" windowWidth="33600" windowHeight="19400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="138">
   <si>
     <t>IMPACT_code</t>
   </si>
@@ -403,16 +403,55 @@
   </si>
   <si>
     <t>11088, 11973, 11304, 16076</t>
+  </si>
+  <si>
+    <t>20076</t>
+  </si>
+  <si>
+    <t>20071</t>
+  </si>
+  <si>
+    <t>20073</t>
+  </si>
+  <si>
+    <t>20074</t>
+  </si>
+  <si>
+    <t>20075</t>
+  </si>
+  <si>
+    <t>20036</t>
+  </si>
+  <si>
+    <t>20040</t>
+  </si>
+  <si>
+    <t>20054</t>
+  </si>
+  <si>
+    <t>20446</t>
+  </si>
+  <si>
+    <t>20450</t>
+  </si>
+  <si>
+    <t>20452</t>
+  </si>
+  <si>
+    <t>20314</t>
+  </si>
+  <si>
+    <t>20014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -515,13 +554,16 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 5" xfId="1"/>
+    <cellStyle name="Normal 5" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -789,21 +831,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A25" sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -814,530 +856,650 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="10">
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C20" s="10">
         <v>69.5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="10">
+        <v>38.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="10">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" s="10">
+        <v>72.900000000000006</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B47" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="10">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="10">
-        <v>38.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+    <row r="48" spans="1:3">
+      <c r="A48" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="10">
-        <v>72.900000000000006</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    <row r="62" spans="1:2">
+      <c r="A62" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C65" s="11">
+        <v>66.67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C40" s="11">
-        <v>66.67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+    <row r="69" spans="1:3">
+      <c r="A69" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+    <row r="71" spans="1:3">
+      <c r="A71" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="10">
-        <v>69.5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" s="10">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B62" s="3"/>
-    </row>
   </sheetData>
+  <sortState ref="A2:C77">
+    <sortCondition ref="A2:A77"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>122</v>
       </c>

</xml_diff>

<commit_message>
ongoing changes to make use of switches work.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/nutrientDetails/IMPACTcodeLookup.xlsx
+++ b/data-raw/NutrientData/nutrientDetails/IMPACTcodeLookup.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutmod/data-raw/NutrientData/nutrientDetails/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988FF599-0743-A242-8113-C55697415DB4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>IMPACT_code</t>
   </si>
@@ -247,12 +248,6 @@
   </si>
   <si>
     <t>11518</t>
-  </si>
-  <si>
-    <t>ctool</t>
-  </si>
-  <si>
-    <t>04670</t>
   </si>
   <si>
     <t>cteas</t>
@@ -695,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -716,15 +711,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C2" s="8">
         <v>69.5</v>
@@ -732,10 +727,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -759,7 +754,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -783,7 +778,7 @@
         <v>34</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -853,7 +848,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C17" s="8">
         <v>82</v>
@@ -941,10 +936,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1000,10 +995,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1064,42 +1059,34 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C43" s="9">
         <v>66.67</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>74</v>
+      <c r="A44" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>80</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C46">
-    <sortCondition ref="A2:A46"/>
+  <sortState ref="A2:C45">
+    <sortCondition ref="A2:A45"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1115,7 +1102,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>